<commit_message>
update for high speed
</commit_message>
<xml_diff>
--- a/input_file.xlsx
+++ b/input_file.xlsx
@@ -6,14 +6,12 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>所属</t>
   </si>
@@ -36,6 +34,9 @@
     <t>くろ</t>
   </si>
   <si>
+    <t>2024/04/01</t>
+  </si>
+  <si>
     <t>国語</t>
   </si>
   <si>
@@ -57,22 +58,42 @@
     <t>ぽち</t>
   </si>
   <si>
+    <t>2024/04/02</t>
+  </si>
+  <si>
+    <t>2024/04/03</t>
+  </si>
+  <si>
     <t>たま</t>
+  </si>
+  <si>
+    <t>2024/05/02</t>
+  </si>
+  <si>
+    <t>2024/05/05</t>
+  </si>
+  <si>
+    <t>2024/05/15</t>
+  </si>
+  <si>
+    <t>2024/06/03</t>
+  </si>
+  <si>
+    <t>2025/03/04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="yyyy/m/d"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="ヒラギノ角ゴ ProN W3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -84,8 +105,14 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="ヒラギノ角ゴ ProN W6"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,8 +125,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -118,6 +157,96 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
@@ -125,33 +254,42 @@
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -170,17 +308,20 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
   <a:themeElements>
-    <a:clrScheme name="Office ​​テーマ">
+    <a:clrScheme name="Blank">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -194,22 +335,22 @@
         <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="00A2FF"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="16E7CF"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="61D836"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFD932"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="FF644E"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="FF42A1"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -218,7 +359,7 @@
         <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office ​​テーマ">
+    <a:fontScheme name="Blank">
       <a:majorFont>
         <a:latin typeface="ヒラギノ角ゴ ProN W6"/>
         <a:ea typeface="ヒラギノ角ゴ ProN W6"/>
@@ -230,7 +371,7 @@
         <a:cs typeface="ヒラギノ角ゴ ProN W3"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office ​​テーマ">
+    <a:fmtScheme name="Blank">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -303,31 +444,13 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -395,16 +518,10 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -680,13 +797,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -961,7 +1072,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1233,17 +1344,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71429" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="8.73438" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.73438" style="1" customWidth="1"/>
+    <col min="1" max="2" width="5.8125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.2109" style="1" customWidth="1"/>
+    <col min="4" max="5" width="5.8125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16" customHeight="1">
+    <row r="1" ht="18.5" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
@@ -1260,394 +1376,212 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="16" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" ht="18.5" customHeight="1">
+      <c r="A2" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="C2" s="3">
-        <v>45383</v>
-      </c>
-      <c r="D2" t="s" s="2">
+      <c r="C2" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="E2" s="4">
+      <c r="D2" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6">
         <v>70</v>
       </c>
     </row>
-    <row r="3" ht="16" customHeight="1">
-      <c r="A3" t="s" s="2">
+    <row r="3" ht="18.3" customHeight="1">
+      <c r="A3" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3">
-        <v>45383</v>
-      </c>
-      <c r="D3" t="s" s="2">
+      <c r="E3" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" ht="18.3" customHeight="1">
+      <c r="A4" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="E3" s="4">
-        <v>80</v>
+      <c r="D4" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10">
+        <v>90</v>
       </c>
     </row>
-    <row r="4" ht="16" customHeight="1">
-      <c r="A4" t="s" s="2">
+    <row r="5" ht="18.3" customHeight="1">
+      <c r="A5" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E5" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" ht="18.3" customHeight="1">
+      <c r="A6" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s" s="9">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E6" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" ht="18.3" customHeight="1">
+      <c r="A7" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E7" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" ht="18.3" customHeight="1">
+      <c r="A8" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E8" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" ht="18.3" customHeight="1">
+      <c r="A9" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s" s="9">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="10">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3">
-        <v>45383</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4">
-        <v>90</v>
-      </c>
     </row>
-    <row r="5" ht="16" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s" s="2">
+    <row r="10" ht="18.3" customHeight="1">
+      <c r="A10" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="C5" s="3">
-        <v>45383</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="B10" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s" s="9">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E10" s="10">
         <v>20</v>
       </c>
     </row>
-    <row r="6" ht="16" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s" s="2">
+    <row r="11" ht="18.3" customHeight="1">
+      <c r="A11" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="C6" s="3">
-        <v>45384</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="B11" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s" s="9">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E11" s="10">
         <v>30</v>
       </c>
     </row>
-    <row r="7" ht="16" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s" s="2">
+    <row r="12" ht="18.3" customHeight="1">
+      <c r="A12" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="C7" s="3">
-        <v>45385</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E7" s="4">
-        <v>40</v>
+      <c r="B12" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E12" s="10">
+        <v>45</v>
       </c>
     </row>
-    <row r="8" ht="16" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3">
-        <v>45383</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" ht="16" customHeight="1">
-      <c r="A9" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C9" s="3">
-        <v>45414</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E9" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" ht="16" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C10" s="3">
-        <v>45417</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" ht="16" customHeight="1">
-      <c r="A11" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3">
-        <v>45427</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" ht="16" customHeight="1">
-      <c r="A12" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3">
-        <v>45446</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" ht="16" customHeight="1">
-      <c r="A13" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3">
-        <v>45720</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E13" s="4">
+    <row r="13" ht="18.3" customHeight="1">
+      <c r="A13" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s" s="9">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E13" s="10">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71429" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="5" width="8.73438" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.73438" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" ht="16" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71429" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="5" width="8.73438" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="8.73438" style="7" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" ht="16" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000&amp;P</oddFooter>

</xml_diff>